<commit_message>
uploaded the python interactive analyzer program
</commit_message>
<xml_diff>
--- a/CB_AI_Programming_Refresher_ILT_Materials_sept/Day wise Agenda/Day_Wise_Agenda_for_Programming_Refresher_3_Hours.xlsx
+++ b/CB_AI_Programming_Refresher_ILT_Materials_sept/Day wise Agenda/Day_Wise_Agenda_for_Programming_Refresher_3_Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2c4e04267d3dad2/Documents/OutoftheNormAi/Simplilearn/CB_AI_Programming_Refresher_ILT_Materials_sept/Day wise Agenda/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2c4e04267d3dad2/Documents/OutoftheNormAi/Simplilearn/simplilearn-AGS/CB_AI_Programming_Refresher_ILT_Materials_sept/Day wise Agenda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="11_1FA6738A85717C41D62200ADA0B88B739A1B1883" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1017ABC6-4778-416A-89B5-48375CEA114A}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="11_1FA6738A85717C41D62200ADA0B88B739A1B1883" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B3A944E-5A42-4BC0-B7E7-494429F44C29}"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="-13068" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Programming Refresher" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -630,13 +630,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -719,7 +739,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -756,20 +776,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -782,24 +789,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1023,7 +1046,7 @@
   <dimension ref="A1:E959"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:E22"/>
+      <selection activeCell="B2" sqref="B2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1053,128 +1076,128 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
+      <c r="A2" s="30">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="21">
         <v>3</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="16" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="16" t="s">
+      <c r="A4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+      <c r="A5" s="30">
         <v>2</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="16" t="s">
+      <c r="A6" s="32"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="16" t="s">
+      <c r="A7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="16" t="s">
+      <c r="A8" s="32"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
+      <c r="A9" s="30">
         <v>3</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="16" t="s">
+      <c r="A10" s="32"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="16" t="s">
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="16" t="s">
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="16" t="s">
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
@@ -1183,146 +1206,146 @@
       <c r="B14" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="21">
         <v>3</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="32" t="s">
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="32" t="s">
+      <c r="A16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="32" t="s">
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="32" t="s">
+      <c r="A18" s="32"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30">
+      <c r="A19" s="26">
         <v>5</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="32" t="s">
+      <c r="A20" s="28"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="32" t="s">
+      <c r="A21" s="28"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="32" t="s">
+      <c r="A22" s="28"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
+      <c r="A23" s="26">
         <v>6</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="21">
         <v>3</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="21">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="16" t="s">
+      <c r="A24" s="28"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="16" t="s">
+      <c r="A25" s="28"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20" t="s">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
@@ -1409,50 +1432,50 @@
       <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="24"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="19"/>
       <c r="C40" s="6"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
-      <c r="B41" s="25"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="20"/>
       <c r="C41" s="6"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
-      <c r="B42" s="25"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="20"/>
       <c r="C42" s="6"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
-      <c r="B43" s="25"/>
+      <c r="A43" s="18"/>
+      <c r="B43" s="20"/>
       <c r="C43" s="6"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
-      <c r="B44" s="25"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="20"/>
       <c r="C44" s="6"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
-      <c r="B45" s="25"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="20"/>
       <c r="C45" s="8"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="25"/>
+      <c r="A46" s="18"/>
+      <c r="B46" s="20"/>
       <c r="C46" s="8"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -5117,13 +5140,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="B40:B46"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A26:A27"/>
     <mergeCell ref="D23:D27"/>
     <mergeCell ref="E23:E27"/>
     <mergeCell ref="A2:A4"/>
@@ -5139,9 +5155,16 @@
     <mergeCell ref="D2:D13"/>
     <mergeCell ref="D14:D22"/>
     <mergeCell ref="E2:E13"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="B40:B46"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A26:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5177,10 +5200,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="22">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5189,42 +5212,42 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26">
+      <c r="A7" s="22">
         <v>2</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="22" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -5233,90 +5256,90 @@
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26">
+      <c r="A18" s="22">
         <v>3</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="25" t="s">
         <v>46</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -5325,162 +5348,162 @@
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="27"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="27"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="23"/>
       <c r="C31" s="5" t="s">
         <v>60</v>
       </c>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
-      <c r="B34" s="27"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="5" t="s">
         <v>63</v>
       </c>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="27"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
       <c r="C35" s="5" t="s">
         <v>64</v>
       </c>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
-      <c r="B36" s="27"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
       <c r="C36" s="5" t="s">
         <v>65</v>
       </c>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
+      <c r="A37" s="24"/>
+      <c r="B37" s="24"/>
       <c r="C37" s="5" t="s">
         <v>66</v>
       </c>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="26">
+      <c r="A38" s="22">
         <v>4</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="25" t="s">
         <v>67</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -5489,58 +5512,58 @@
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
-      <c r="B39" s="27"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
       <c r="C39" s="5" t="s">
         <v>64</v>
       </c>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
-      <c r="B40" s="27"/>
+      <c r="A40" s="23"/>
+      <c r="B40" s="23"/>
       <c r="C40" s="5" t="s">
         <v>69</v>
       </c>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
-      <c r="B41" s="27"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="23"/>
       <c r="C41" s="5" t="s">
         <v>70</v>
       </c>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
-      <c r="B42" s="27"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="23"/>
       <c r="C42" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="5" t="s">
         <v>72</v>
       </c>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="24"/>
       <c r="C44" s="5" t="s">
         <v>73</v>
       </c>
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="26">
+      <c r="A45" s="22">
         <v>5</v>
       </c>
-      <c r="B45" s="29" t="s">
+      <c r="B45" s="25" t="s">
         <v>74</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -5549,98 +5572,98 @@
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="27"/>
-      <c r="B46" s="27"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="5" t="s">
         <v>76</v>
       </c>
       <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="27"/>
-      <c r="B47" s="27"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="23"/>
       <c r="C47" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="27"/>
-      <c r="B48" s="27"/>
+      <c r="A48" s="23"/>
+      <c r="B48" s="23"/>
       <c r="C48" s="5" t="s">
         <v>78</v>
       </c>
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
-      <c r="B49" s="27"/>
+      <c r="A49" s="23"/>
+      <c r="B49" s="23"/>
       <c r="C49" s="5" t="s">
         <v>79</v>
       </c>
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="27"/>
-      <c r="B50" s="27"/>
+      <c r="A50" s="23"/>
+      <c r="B50" s="23"/>
       <c r="C50" s="5" t="s">
         <v>80</v>
       </c>
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="27"/>
-      <c r="B51" s="27"/>
+      <c r="A51" s="23"/>
+      <c r="B51" s="23"/>
       <c r="C51" s="5" t="s">
         <v>81</v>
       </c>
       <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="27"/>
-      <c r="B52" s="27"/>
+      <c r="A52" s="23"/>
+      <c r="B52" s="23"/>
       <c r="C52" s="5" t="s">
         <v>82</v>
       </c>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="27"/>
-      <c r="B53" s="27"/>
+      <c r="A53" s="23"/>
+      <c r="B53" s="23"/>
       <c r="C53" s="5" t="s">
         <v>83</v>
       </c>
       <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="27"/>
-      <c r="B54" s="27"/>
+      <c r="A54" s="23"/>
+      <c r="B54" s="23"/>
       <c r="C54" s="5" t="s">
         <v>84</v>
       </c>
       <c r="D54" s="2"/>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="27"/>
-      <c r="B55" s="27"/>
+      <c r="A55" s="23"/>
+      <c r="B55" s="23"/>
       <c r="C55" s="5" t="s">
         <v>85</v>
       </c>
       <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="28"/>
-      <c r="B56" s="28"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="24"/>
       <c r="C56" s="5" t="s">
         <v>86</v>
       </c>
       <c r="D56" s="2"/>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="26">
+      <c r="A57" s="22">
         <v>6</v>
       </c>
-      <c r="B57" s="29" t="s">
+      <c r="B57" s="25" t="s">
         <v>87</v>
       </c>
       <c r="C57" s="5" t="s">
@@ -5649,74 +5672,74 @@
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="27"/>
-      <c r="B58" s="27"/>
+      <c r="A58" s="23"/>
+      <c r="B58" s="23"/>
       <c r="C58" s="5" t="s">
         <v>89</v>
       </c>
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="27"/>
-      <c r="B59" s="27"/>
+      <c r="A59" s="23"/>
+      <c r="B59" s="23"/>
       <c r="C59" s="5" t="s">
         <v>90</v>
       </c>
       <c r="D59" s="2"/>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="27"/>
-      <c r="B60" s="27"/>
+      <c r="A60" s="23"/>
+      <c r="B60" s="23"/>
       <c r="C60" s="5" t="s">
         <v>91</v>
       </c>
       <c r="D60" s="2"/>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="27"/>
-      <c r="B61" s="27"/>
+      <c r="A61" s="23"/>
+      <c r="B61" s="23"/>
       <c r="C61" s="5" t="s">
         <v>92</v>
       </c>
       <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="27"/>
-      <c r="B62" s="27"/>
+      <c r="A62" s="23"/>
+      <c r="B62" s="23"/>
       <c r="C62" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="27"/>
-      <c r="B63" s="27"/>
+      <c r="A63" s="23"/>
+      <c r="B63" s="23"/>
       <c r="C63" s="5" t="s">
         <v>94</v>
       </c>
       <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="27"/>
-      <c r="B64" s="27"/>
+      <c r="A64" s="23"/>
+      <c r="B64" s="23"/>
       <c r="C64" s="5" t="s">
         <v>95</v>
       </c>
       <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="28"/>
-      <c r="B65" s="28"/>
+      <c r="A65" s="24"/>
+      <c r="B65" s="24"/>
       <c r="C65" s="5" t="s">
         <v>96</v>
       </c>
       <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="26">
+      <c r="A66" s="22">
         <v>7</v>
       </c>
-      <c r="B66" s="29" t="s">
+      <c r="B66" s="25" t="s">
         <v>97</v>
       </c>
       <c r="C66" s="5" t="s">
@@ -5725,26 +5748,26 @@
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="27"/>
-      <c r="B67" s="27"/>
+      <c r="A67" s="23"/>
+      <c r="B67" s="23"/>
       <c r="C67" s="5" t="s">
         <v>99</v>
       </c>
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="28"/>
-      <c r="B68" s="28"/>
+      <c r="A68" s="24"/>
+      <c r="B68" s="24"/>
       <c r="C68" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="26">
+      <c r="A69" s="22">
         <v>8</v>
       </c>
-      <c r="B69" s="29" t="s">
+      <c r="B69" s="25" t="s">
         <v>101</v>
       </c>
       <c r="C69" s="5" t="s">
@@ -5753,42 +5776,42 @@
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="27"/>
-      <c r="B70" s="27"/>
+      <c r="A70" s="23"/>
+      <c r="B70" s="23"/>
       <c r="C70" s="5" t="s">
         <v>103</v>
       </c>
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="27"/>
-      <c r="B71" s="27"/>
+      <c r="A71" s="23"/>
+      <c r="B71" s="23"/>
       <c r="C71" s="5" t="s">
         <v>104</v>
       </c>
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="27"/>
-      <c r="B72" s="27"/>
+      <c r="A72" s="23"/>
+      <c r="B72" s="23"/>
       <c r="C72" s="5" t="s">
         <v>105</v>
       </c>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="28"/>
-      <c r="B73" s="28"/>
+      <c r="A73" s="24"/>
+      <c r="B73" s="24"/>
       <c r="C73" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="26">
+      <c r="A74" s="22">
         <v>9</v>
       </c>
-      <c r="B74" s="29" t="s">
+      <c r="B74" s="25" t="s">
         <v>107</v>
       </c>
       <c r="C74" s="5" t="s">
@@ -5797,26 +5820,26 @@
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="27"/>
-      <c r="B75" s="27"/>
+      <c r="A75" s="23"/>
+      <c r="B75" s="23"/>
       <c r="C75" s="5" t="s">
         <v>109</v>
       </c>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="28"/>
-      <c r="B76" s="28"/>
+      <c r="A76" s="24"/>
+      <c r="B76" s="24"/>
       <c r="C76" s="5" t="s">
         <v>110</v>
       </c>
       <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="26">
+      <c r="A77" s="22">
         <v>10</v>
       </c>
-      <c r="B77" s="29" t="s">
+      <c r="B77" s="25" t="s">
         <v>111</v>
       </c>
       <c r="C77" s="5" t="s">
@@ -5825,82 +5848,82 @@
       <c r="D77" s="2"/>
     </row>
     <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="27"/>
-      <c r="B78" s="27"/>
+      <c r="A78" s="23"/>
+      <c r="B78" s="23"/>
       <c r="C78" s="5" t="s">
         <v>113</v>
       </c>
       <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="27"/>
-      <c r="B79" s="27"/>
+      <c r="A79" s="23"/>
+      <c r="B79" s="23"/>
       <c r="C79" s="5" t="s">
         <v>114</v>
       </c>
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="27"/>
-      <c r="B80" s="27"/>
+      <c r="A80" s="23"/>
+      <c r="B80" s="23"/>
       <c r="C80" s="5" t="s">
         <v>115</v>
       </c>
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="27"/>
-      <c r="B81" s="27"/>
+      <c r="A81" s="23"/>
+      <c r="B81" s="23"/>
       <c r="C81" s="5" t="s">
         <v>116</v>
       </c>
       <c r="D81" s="2"/>
     </row>
     <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="27"/>
-      <c r="B82" s="27"/>
+      <c r="A82" s="23"/>
+      <c r="B82" s="23"/>
       <c r="C82" s="5" t="s">
         <v>117</v>
       </c>
       <c r="D82" s="2"/>
     </row>
     <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="27"/>
-      <c r="B83" s="27"/>
+      <c r="A83" s="23"/>
+      <c r="B83" s="23"/>
       <c r="C83" s="5" t="s">
         <v>118</v>
       </c>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="27"/>
-      <c r="B84" s="27"/>
+      <c r="A84" s="23"/>
+      <c r="B84" s="23"/>
       <c r="C84" s="5" t="s">
         <v>119</v>
       </c>
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="27"/>
-      <c r="B85" s="27"/>
+      <c r="A85" s="23"/>
+      <c r="B85" s="23"/>
       <c r="C85" s="5" t="s">
         <v>120</v>
       </c>
       <c r="D85" s="2"/>
     </row>
     <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="28"/>
-      <c r="B86" s="28"/>
+      <c r="A86" s="24"/>
+      <c r="B86" s="24"/>
       <c r="C86" s="5" t="s">
         <v>121</v>
       </c>
       <c r="D86" s="2"/>
     </row>
     <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="26">
+      <c r="A87" s="22">
         <v>11</v>
       </c>
-      <c r="B87" s="29" t="s">
+      <c r="B87" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C87" s="5" t="s">
@@ -5909,130 +5932,130 @@
       <c r="D87" s="2"/>
     </row>
     <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="27"/>
-      <c r="B88" s="27"/>
+      <c r="A88" s="23"/>
+      <c r="B88" s="23"/>
       <c r="C88" s="5" t="s">
         <v>124</v>
       </c>
       <c r="D88" s="2"/>
     </row>
     <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="27"/>
-      <c r="B89" s="27"/>
+      <c r="A89" s="23"/>
+      <c r="B89" s="23"/>
       <c r="C89" s="5" t="s">
         <v>125</v>
       </c>
       <c r="D89" s="2"/>
     </row>
     <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="27"/>
-      <c r="B90" s="27"/>
+      <c r="A90" s="23"/>
+      <c r="B90" s="23"/>
       <c r="C90" s="5" t="s">
         <v>126</v>
       </c>
       <c r="D90" s="2"/>
     </row>
     <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="27"/>
-      <c r="B91" s="27"/>
+      <c r="A91" s="23"/>
+      <c r="B91" s="23"/>
       <c r="C91" s="5" t="s">
         <v>127</v>
       </c>
       <c r="D91" s="2"/>
     </row>
     <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="27"/>
-      <c r="B92" s="27"/>
+      <c r="A92" s="23"/>
+      <c r="B92" s="23"/>
       <c r="C92" s="5" t="s">
         <v>128</v>
       </c>
       <c r="D92" s="2"/>
     </row>
     <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="27"/>
-      <c r="B93" s="27"/>
+      <c r="A93" s="23"/>
+      <c r="B93" s="23"/>
       <c r="C93" s="5" t="s">
         <v>129</v>
       </c>
       <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="27"/>
-      <c r="B94" s="27"/>
+      <c r="A94" s="23"/>
+      <c r="B94" s="23"/>
       <c r="C94" s="5" t="s">
         <v>130</v>
       </c>
       <c r="D94" s="2"/>
     </row>
     <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="27"/>
-      <c r="B95" s="27"/>
+      <c r="A95" s="23"/>
+      <c r="B95" s="23"/>
       <c r="C95" s="5" t="s">
         <v>131</v>
       </c>
       <c r="D95" s="2"/>
     </row>
     <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="27"/>
-      <c r="B96" s="27"/>
+      <c r="A96" s="23"/>
+      <c r="B96" s="23"/>
       <c r="C96" s="5" t="s">
         <v>132</v>
       </c>
       <c r="D96" s="2"/>
     </row>
     <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="27"/>
-      <c r="B97" s="27"/>
+      <c r="A97" s="23"/>
+      <c r="B97" s="23"/>
       <c r="C97" s="5" t="s">
         <v>133</v>
       </c>
       <c r="D97" s="2"/>
     </row>
     <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="27"/>
-      <c r="B98" s="27"/>
+      <c r="A98" s="23"/>
+      <c r="B98" s="23"/>
       <c r="C98" s="5" t="s">
         <v>134</v>
       </c>
       <c r="D98" s="2"/>
     </row>
     <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="27"/>
-      <c r="B99" s="27"/>
+      <c r="A99" s="23"/>
+      <c r="B99" s="23"/>
       <c r="C99" s="5" t="s">
         <v>135</v>
       </c>
       <c r="D99" s="2"/>
     </row>
     <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="27"/>
-      <c r="B100" s="27"/>
+      <c r="A100" s="23"/>
+      <c r="B100" s="23"/>
       <c r="C100" s="5" t="s">
         <v>136</v>
       </c>
       <c r="D100" s="2"/>
     </row>
     <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="27"/>
-      <c r="B101" s="27"/>
+      <c r="A101" s="23"/>
+      <c r="B101" s="23"/>
       <c r="C101" s="5" t="s">
         <v>137</v>
       </c>
       <c r="D101" s="2"/>
     </row>
     <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="28"/>
-      <c r="B102" s="28"/>
+      <c r="A102" s="24"/>
+      <c r="B102" s="24"/>
       <c r="C102" s="5" t="s">
         <v>138</v>
       </c>
       <c r="D102" s="2"/>
     </row>
     <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="26">
+      <c r="A103" s="22">
         <v>12</v>
       </c>
-      <c r="B103" s="29" t="s">
+      <c r="B103" s="25" t="s">
         <v>139</v>
       </c>
       <c r="C103" s="5" t="s">
@@ -6041,106 +6064,106 @@
       <c r="D103" s="2"/>
     </row>
     <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="27"/>
-      <c r="B104" s="27"/>
+      <c r="A104" s="23"/>
+      <c r="B104" s="23"/>
       <c r="C104" s="5" t="s">
         <v>141</v>
       </c>
       <c r="D104" s="2"/>
     </row>
     <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="27"/>
-      <c r="B105" s="27"/>
+      <c r="A105" s="23"/>
+      <c r="B105" s="23"/>
       <c r="C105" s="5" t="s">
         <v>142</v>
       </c>
       <c r="D105" s="2"/>
     </row>
     <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="27"/>
-      <c r="B106" s="27"/>
+      <c r="A106" s="23"/>
+      <c r="B106" s="23"/>
       <c r="C106" s="5" t="s">
         <v>143</v>
       </c>
       <c r="D106" s="2"/>
     </row>
     <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="27"/>
-      <c r="B107" s="27"/>
+      <c r="A107" s="23"/>
+      <c r="B107" s="23"/>
       <c r="C107" s="5" t="s">
         <v>144</v>
       </c>
       <c r="D107" s="2"/>
     </row>
     <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="27"/>
-      <c r="B108" s="27"/>
+      <c r="A108" s="23"/>
+      <c r="B108" s="23"/>
       <c r="C108" s="5" t="s">
         <v>145</v>
       </c>
       <c r="D108" s="2"/>
     </row>
     <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="27"/>
-      <c r="B109" s="27"/>
+      <c r="A109" s="23"/>
+      <c r="B109" s="23"/>
       <c r="C109" s="5" t="s">
         <v>146</v>
       </c>
       <c r="D109" s="2"/>
     </row>
     <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="27"/>
-      <c r="B110" s="27"/>
+      <c r="A110" s="23"/>
+      <c r="B110" s="23"/>
       <c r="C110" s="5" t="s">
         <v>147</v>
       </c>
       <c r="D110" s="2"/>
     </row>
     <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="27"/>
-      <c r="B111" s="27"/>
+      <c r="A111" s="23"/>
+      <c r="B111" s="23"/>
       <c r="C111" s="5" t="s">
         <v>148</v>
       </c>
       <c r="D111" s="2"/>
     </row>
     <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="27"/>
-      <c r="B112" s="27"/>
+      <c r="A112" s="23"/>
+      <c r="B112" s="23"/>
       <c r="C112" s="5" t="s">
         <v>149</v>
       </c>
       <c r="D112" s="2"/>
     </row>
     <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="27"/>
-      <c r="B113" s="27"/>
+      <c r="A113" s="23"/>
+      <c r="B113" s="23"/>
       <c r="C113" s="5" t="s">
         <v>150</v>
       </c>
       <c r="D113" s="2"/>
     </row>
     <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="27"/>
-      <c r="B114" s="27"/>
+      <c r="A114" s="23"/>
+      <c r="B114" s="23"/>
       <c r="C114" s="5" t="s">
         <v>151</v>
       </c>
       <c r="D114" s="2"/>
     </row>
     <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="28"/>
-      <c r="B115" s="28"/>
+      <c r="A115" s="24"/>
+      <c r="B115" s="24"/>
       <c r="C115" s="5" t="s">
         <v>152</v>
       </c>
       <c r="D115" s="2"/>
     </row>
     <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="26">
+      <c r="A116" s="22">
         <v>13</v>
       </c>
-      <c r="B116" s="29" t="s">
+      <c r="B116" s="25" t="s">
         <v>153</v>
       </c>
       <c r="C116" s="5" t="s">
@@ -6149,58 +6172,58 @@
       <c r="D116" s="2"/>
     </row>
     <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="27"/>
-      <c r="B117" s="27"/>
+      <c r="A117" s="23"/>
+      <c r="B117" s="23"/>
       <c r="C117" s="5" t="s">
         <v>155</v>
       </c>
       <c r="D117" s="2"/>
     </row>
     <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="27"/>
-      <c r="B118" s="27"/>
+      <c r="A118" s="23"/>
+      <c r="B118" s="23"/>
       <c r="C118" s="5" t="s">
         <v>156</v>
       </c>
       <c r="D118" s="2"/>
     </row>
     <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="27"/>
-      <c r="B119" s="27"/>
+      <c r="A119" s="23"/>
+      <c r="B119" s="23"/>
       <c r="C119" s="5" t="s">
         <v>157</v>
       </c>
       <c r="D119" s="2"/>
     </row>
     <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="27"/>
-      <c r="B120" s="27"/>
+      <c r="A120" s="23"/>
+      <c r="B120" s="23"/>
       <c r="C120" s="5" t="s">
         <v>158</v>
       </c>
       <c r="D120" s="2"/>
     </row>
     <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="27"/>
-      <c r="B121" s="27"/>
+      <c r="A121" s="23"/>
+      <c r="B121" s="23"/>
       <c r="C121" s="5" t="s">
         <v>159</v>
       </c>
       <c r="D121" s="2"/>
     </row>
     <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="28"/>
-      <c r="B122" s="28"/>
+      <c r="A122" s="24"/>
+      <c r="B122" s="24"/>
       <c r="C122" s="5" t="s">
         <v>160</v>
       </c>
       <c r="D122" s="2"/>
     </row>
     <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="26">
+      <c r="A123" s="22">
         <v>14</v>
       </c>
-      <c r="B123" s="29" t="s">
+      <c r="B123" s="25" t="s">
         <v>161</v>
       </c>
       <c r="C123" s="5" t="s">
@@ -6209,56 +6232,56 @@
       <c r="D123" s="2"/>
     </row>
     <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="27"/>
-      <c r="B124" s="27"/>
+      <c r="A124" s="23"/>
+      <c r="B124" s="23"/>
       <c r="C124" s="5" t="s">
         <v>163</v>
       </c>
       <c r="D124" s="2"/>
     </row>
     <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="27"/>
-      <c r="B125" s="27"/>
+      <c r="A125" s="23"/>
+      <c r="B125" s="23"/>
       <c r="C125" s="5" t="s">
         <v>164</v>
       </c>
       <c r="D125" s="2"/>
     </row>
     <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="27"/>
-      <c r="B126" s="27"/>
+      <c r="A126" s="23"/>
+      <c r="B126" s="23"/>
       <c r="C126" s="5" t="s">
         <v>165</v>
       </c>
       <c r="D126" s="2"/>
     </row>
     <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="27"/>
-      <c r="B127" s="27"/>
+      <c r="A127" s="23"/>
+      <c r="B127" s="23"/>
       <c r="C127" s="5" t="s">
         <v>166</v>
       </c>
       <c r="D127" s="2"/>
     </row>
     <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="27"/>
-      <c r="B128" s="27"/>
+      <c r="A128" s="23"/>
+      <c r="B128" s="23"/>
       <c r="C128" s="5" t="s">
         <v>167</v>
       </c>
       <c r="D128" s="2"/>
     </row>
     <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="28"/>
-      <c r="B129" s="28"/>
+      <c r="A129" s="24"/>
+      <c r="B129" s="24"/>
       <c r="C129" s="5" t="s">
         <v>168</v>
       </c>
       <c r="D129" s="2"/>
     </row>
     <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="26"/>
-      <c r="B130" s="26" t="s">
+      <c r="A130" s="22"/>
+      <c r="B130" s="22" t="s">
         <v>169</v>
       </c>
       <c r="C130" s="2" t="s">
@@ -6267,8 +6290,8 @@
       <c r="D130" s="2"/>
     </row>
     <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="28"/>
-      <c r="B131" s="28"/>
+      <c r="A131" s="24"/>
+      <c r="B131" s="24"/>
       <c r="C131" s="2" t="s">
         <v>171</v>
       </c>
@@ -7145,12 +7168,18 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A123:A129"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="B103:B115"/>
-    <mergeCell ref="B116:B122"/>
-    <mergeCell ref="B123:B129"/>
-    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A7:A17"/>
+    <mergeCell ref="B7:B17"/>
+    <mergeCell ref="A18:A37"/>
+    <mergeCell ref="B18:B37"/>
+    <mergeCell ref="B38:B44"/>
+    <mergeCell ref="A38:A44"/>
+    <mergeCell ref="A45:A56"/>
+    <mergeCell ref="B45:B56"/>
+    <mergeCell ref="A57:A65"/>
+    <mergeCell ref="B57:B65"/>
     <mergeCell ref="A66:A68"/>
     <mergeCell ref="B66:B68"/>
     <mergeCell ref="A87:A102"/>
@@ -7163,18 +7192,12 @@
     <mergeCell ref="A77:A86"/>
     <mergeCell ref="B77:B86"/>
     <mergeCell ref="B87:B102"/>
-    <mergeCell ref="B38:B44"/>
-    <mergeCell ref="A38:A44"/>
-    <mergeCell ref="A45:A56"/>
-    <mergeCell ref="B45:B56"/>
-    <mergeCell ref="A57:A65"/>
-    <mergeCell ref="B57:B65"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A7:A17"/>
-    <mergeCell ref="B7:B17"/>
-    <mergeCell ref="A18:A37"/>
-    <mergeCell ref="B18:B37"/>
+    <mergeCell ref="A123:A129"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="B103:B115"/>
+    <mergeCell ref="B116:B122"/>
+    <mergeCell ref="B123:B129"/>
+    <mergeCell ref="B130:B131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>